<commit_message>
[ADD] Added entity and table classes for java application and .xlsx files for data import
</commit_message>
<xml_diff>
--- a/table import/organismi.xlsx
+++ b/table import/organismi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Atolla wyvillei</t>
   </si>
   <si>
-    <t xml:space="preserve">Questa specie di medusa presenta una corona rossa</t>
+    <t xml:space="preserve">Questa specie di medusa presenta una campana rossa e un lungo tentacolo bianco che parte dal centro della campana e si allunga per una decina di centimetri</t>
   </si>
   <si>
     <t xml:space="preserve">A69M3QUS9A</t>
@@ -85,16 +85,55 @@
     <t xml:space="preserve">KHRIIMYK0J</t>
   </si>
   <si>
+    <t xml:space="preserve">Marrus orthocana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medusa sifonofora cintura di fuoco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questa specie di sifonoforo presenta un colore rosso/arancio intenso, essendo i sifonofori dei raggruppamenti di organismi, può assumere diverse forme, caratterizzate solitamente da filamenti intrecciati.</t>
+  </si>
+  <si>
     <t xml:space="preserve">P4FPZBSA8O</t>
   </si>
   <si>
+    <t xml:space="preserve">Solmissus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medusa piatto da cena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questa specie di medusa presenta numerosi e sottili tentacoli. La campana è quasi completamente trasparente. Sia i tentacoli che la campana sono fluorescenti e di colore bianco/azzurro.</t>
+  </si>
+  <si>
     <t xml:space="preserve">0F5W9M2W7L</t>
   </si>
   <si>
+    <t xml:space="preserve">Tiburonia granrojo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grande medusa rossa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il nome di questa medusa deriva dai suoi colori rossi della campana (granrojo = grande rosso in spagnolo). Presenta una campana di grandi dimensioni, mentre i tentacoli sono più corti e tozzi.</t>
+  </si>
+  <si>
     <t xml:space="preserve">AI4CEQC9PM</t>
   </si>
   <si>
+    <t xml:space="preserve">Medusa quadri-tentacolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questa medusa di piccole dimensioni presenta 4 sottili tentacoli e una campana trasparente con un anello fluorescente. Utilizza la propulsione causata dal movimento della campana per muoversi.</t>
+  </si>
+  <si>
     <t xml:space="preserve">6567LBSV3P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larvacean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I larvacei sono tunicati che abitano diverse zone degli oceani di tutto il mondo, per nutrirsi utilizzano una “barriera” di muco che filtra le sostanze nutritive.</t>
   </si>
   <si>
     <t xml:space="preserve">ORYC2H5PF4</t>
@@ -142,6 +181,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -163,11 +203,13 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -315,23 +357,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="98.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="98.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -385,7 +427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -419,54 +461,94 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -475,7 +557,7 @@
     </row>
     <row r="12" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -484,7 +566,7 @@
     </row>
     <row r="13" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -493,7 +575,7 @@
     </row>
     <row r="14" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -502,7 +584,7 @@
     </row>
     <row r="15" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -511,7 +593,7 @@
     </row>
     <row r="16" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -520,7 +602,7 @@
     </row>
     <row r="17" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -529,7 +611,7 @@
     </row>
     <row r="18" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -538,7 +620,7 @@
     </row>
     <row r="19" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -547,7 +629,7 @@
     </row>
     <row r="20" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -556,7 +638,7 @@
     </row>
     <row r="21" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>

</xml_diff>

<commit_message>
[MOD] Modified address field in database, added associations and manufacturers. Added organisms to excel file
</commit_message>
<xml_diff>
--- a/table import/organismi.xlsx
+++ b/table import/organismi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -139,28 +139,97 @@
     <t xml:space="preserve">ORYC2H5PF4</t>
   </si>
   <si>
+    <t xml:space="preserve">Albatrossia pectoralis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coda di ratto gigante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questo pesce è solito abitare il suolo marino. Possiede una corporatura tozza con una coda più sottile. Esemplari di questa specie possono crescere anche fino a 2 metri di lunghezza.</t>
+  </si>
+  <si>
     <t xml:space="preserve">JANN0QNIG4</t>
   </si>
   <si>
+    <t xml:space="preserve">Psychrolutes phrictus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blob sculpin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questa specie di sculpin abita le profondità più oscure degli oceani. Presentano diverse spine, come tutte le altre specie di sculpin, ma presentano anche una corporatura più tozza.</t>
+  </si>
+  <si>
     <t xml:space="preserve">VL5L84606R</t>
   </si>
   <si>
+    <t xml:space="preserve">Gambero pesante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questa specie di gambero utilizza una dura corazza per proteggersi; questo comporta un maggiore peso, che non gli permette di nuotare come altre specie di gamberetti. Saranno necessari ulteriori studi.</t>
+  </si>
+  <si>
     <t xml:space="preserve">WOCOAYY52M</t>
   </si>
   <si>
+    <t xml:space="preserve">Pycnogonid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ragno marino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questi artropodi sono stati osservati a profondità elevate, gli esemplari possono essere di colore diverso e tutti posseggono otto zampe sottili, come i ragni comuni, e un torso piccolo.</t>
+  </si>
+  <si>
     <t xml:space="preserve">7F0JSTSGR0</t>
   </si>
   <si>
+    <t xml:space="preserve">Magnapinna atlantica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questi calamari sono caratterizzati, come gli altri membri del loro genere, da tentacoli molto lunghi, anche fino a 8 metri. Abitano le zone più profonde e oscure degli oceani, ancora non si sa di cosa si nutrono e le loro abitudini.</t>
+  </si>
+  <si>
     <t xml:space="preserve">EAU993XFSA</t>
   </si>
   <si>
+    <t xml:space="preserve">Deepstaria enigmatica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queste meduse sono solite abitare profondità elevate. Possiedono una larga ma sottile campana trasparente, che può raggiungere anche i 2 metri di larghezza. Non possiedono tentacoli e vivono in solitudine.</t>
+  </si>
+  <si>
     <t xml:space="preserve">VKFBS2ECGG</t>
   </si>
   <si>
+    <t xml:space="preserve">Periphyllopsis braueri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queste meduse presentano una campana spessa e di colore grigio/viola. I tentacoli sono molto sottili e genericamente di colore bianco. La campana presenta inoltre delle appendici che si muovono come i petali di un fiore, chiudendosi concentricamente per spingersi in avanti.</t>
+  </si>
+  <si>
     <t xml:space="preserve">WOXO3HBSWG</t>
   </si>
   <si>
+    <t xml:space="preserve">Hexanchus griseus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Squalo vacca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questo squalo presenta 6 paia di branchie e un muso schiacciato. Possono crescere fino a 6 metri di lunghezza.</t>
+  </si>
+  <si>
     <t xml:space="preserve">LBPHU6GZV0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enypniastes eximia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danzatore spagnolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questa specie di cetriolo marino nuota a profondità elevate. Presenta una colorazione accesa, solitamente rosso, rosa o arancione.</t>
   </si>
   <si>
     <t xml:space="preserve">EZH5BFUT5O</t>
@@ -267,20 +336,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,349 +430,419 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="98.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="98.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+    <row r="11" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="A20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="A21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[MOD] Adjusted size for text fields and scrollpane
</commit_message>
<xml_diff>
--- a/table import/organismi.xlsx
+++ b/table import/organismi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -43,9 +43,6 @@
     <t xml:space="preserve">Taonius borealis</t>
   </si>
   <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
     <t xml:space="preserve">Calamaro cacatua</t>
   </si>
   <si>
@@ -73,13 +70,13 @@
     <t xml:space="preserve">A69M3QUS9A</t>
   </si>
   <si>
-    <t xml:space="preserve">Ctenophore</t>
+    <t xml:space="preserve">Beroe forskalii</t>
   </si>
   <si>
     <t xml:space="preserve">Medusa pettine</t>
   </si>
   <si>
-    <t xml:space="preserve">Questa specie di medusa di piccole dimensioni presenta un corpo completamente trasparente, fatta eccezione di filamenti “dentati” all’interno del corpo</t>
+    <t xml:space="preserve">Questa specie di ctenoforo di piccole dimensioni presenta un corpo completamente trasparente, fatta eccezione di filamenti “dentati” all’interno del corpo</t>
   </si>
   <si>
     <t xml:space="preserve">KHRIIMYK0J</t>
@@ -235,7 +232,25 @@
     <t xml:space="preserve">EZH5BFUT5O</t>
   </si>
   <si>
+    <t xml:space="preserve">Lampocteis cruentiventer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctenoforo dal ventre insanguinato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questo ctenoforo presenta un colore rosso molto intenso e dei filamenti interni seghettati che vengono talvolta attraversati da particelle bio-luminose sconosciute. Al momento sono l’unica specie conosciuta del loro genere.</t>
+  </si>
+  <si>
     <t xml:space="preserve">83SIM574N8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexatrygon bickelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Razza esabranchiata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questa specie di razza presenta 6 paia di branchie, da cui deriva il suo nome. La testa è allungata e le dimensioni totali possono raggiungere anche 1.7m. Solitamente vivono a stretto contatto con il fondale marino.</t>
   </si>
 </sst>
 </file>
@@ -437,7 +452,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -473,320 +488,282 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="3" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="3" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>

</xml_diff>